<commit_message>
Pequena falha no cronograma fixada.
</commit_message>
<xml_diff>
--- a/Apresentaçao Final/Cronograma.xlsx
+++ b/Apresentaçao Final/Cronograma.xlsx
@@ -4378,10 +4378,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:W24"/>
+  <dimension ref="B2:W22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X19" activeCellId="0" sqref="X19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N24" activeCellId="0" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33.75"/>
@@ -4871,11 +4871,6 @@
       <c r="U22" s="23"/>
       <c r="V22" s="23"/>
       <c r="W22" s="23"/>
-    </row>
-    <row r="24" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N24" s="0" t="n">
-        <v>12</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
Repositório limpo. E explicações sobre o uso de imagens adicionado.
</commit_message>
<xml_diff>
--- a/Apresentaçao Final/Cronograma.xlsx
+++ b/Apresentaçao Final/Cronograma.xlsx
@@ -4378,10 +4378,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:W24"/>
+  <dimension ref="B2:W22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X19" activeCellId="0" sqref="X19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N24" activeCellId="0" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33.75"/>
@@ -4871,11 +4871,6 @@
       <c r="U22" s="23"/>
       <c r="V22" s="23"/>
       <c r="W22" s="23"/>
-    </row>
-    <row r="24" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N24" s="0" t="n">
-        <v>12</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>